<commit_message>
working on multi threads
</commit_message>
<xml_diff>
--- a/streetstat/assets/report/report.xlsx
+++ b/streetstat/assets/report/report.xlsx
@@ -467,36 +467,36 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>5</v>
+        <v>200</v>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>10</v>
+        <v>205</v>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -507,16 +507,16 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>15</v>
+        <v>210</v>
       </c>
       <c r="B4" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D4" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -527,36 +527,36 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>20</v>
+        <v>215</v>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C5" t="n">
         <v>3</v>
       </c>
       <c r="D5" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>25</v>
+        <v>220</v>
       </c>
       <c r="B6" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C6" t="n">
         <v>3</v>
       </c>
       <c r="D6" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -567,16 +567,16 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>30</v>
+        <v>225</v>
       </c>
       <c r="B7" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>

</xml_diff>